<commit_message>
updated with another measurement data
</commit_message>
<xml_diff>
--- a/Distance measurements.xlsx
+++ b/Distance measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7130" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="7130"/>
   </bookViews>
   <sheets>
     <sheet name="Distance Measurements" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Joint1</t>
   </si>
@@ -26,7 +26,10 @@
     <t>Joint3</t>
   </si>
   <si>
-    <t>Measured</t>
+    <t>Measured2</t>
+  </si>
+  <si>
+    <t>Measured1</t>
   </si>
   <si>
     <t>matlab</t>
@@ -717,7 +720,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -725,6 +728,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1046,18 +1052,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="12.9090909090909" customWidth="1"/>
+    <col min="5" max="6" width="10.6363636363636" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1074,10 +1081,13 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1088,16 +1098,19 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
+        <v>0.212</v>
+      </c>
+      <c r="F2" s="3">
         <v>0.198</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>0.2047</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -1108,16 +1121,19 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
+        <v>0.115</v>
+      </c>
+      <c r="F3" s="3">
         <v>0.107</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>0.1095</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -1128,16 +1144,19 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
+        <v>0.233</v>
+      </c>
+      <c r="F4" s="3">
         <v>0.23</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0.2273</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>90</v>
@@ -1148,16 +1167,19 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
+        <v>0.118</v>
+      </c>
+      <c r="F5" s="3">
         <v>0.11</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0.1119</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>90</v>
@@ -1168,16 +1190,19 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
+        <v>0.087</v>
+      </c>
+      <c r="F6" s="3">
         <v>0.075</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0.07868</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>90</v>
@@ -1188,16 +1213,19 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>0.136</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
+        <v>0.136</v>
+      </c>
+      <c r="G7" s="2">
         <v>0.1296</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>-90</v>
@@ -1208,16 +1236,19 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>0.264</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
+        <v>0.264</v>
+      </c>
+      <c r="G8" s="2">
         <v>0.2576</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>-90</v>
@@ -1228,16 +1259,19 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>0.175</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
+        <v>0.175</v>
+      </c>
+      <c r="G9" s="2">
         <v>0.1759</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>-90</v>
@@ -1248,10 +1282,13 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
+        <v>0.231</v>
+      </c>
+      <c r="F10" s="3">
         <v>0.237</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>0.2292</v>
       </c>
     </row>
@@ -1266,30 +1303,30 @@
   <sheetPr/>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="2:7">
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1351,6 +1388,9 @@
       <c r="D4">
         <v>0.02</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="F4">
         <v>0</v>
       </c>
@@ -1360,7 +1400,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <f>C9/E9</f>
@@ -1394,7 +1434,7 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>2.2</v>

</xml_diff>

<commit_message>
optimize all DH parameters and offset, base X,Y,Z
</commit_message>
<xml_diff>
--- a/Distance measurements.xlsx
+++ b/Distance measurements.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Joint1</t>
   </si>
@@ -29,13 +29,15 @@
     <t>Measured</t>
   </si>
   <si>
-    <t>Calculated</t>
+    <t>Before Optimization
+Calculated</t>
   </si>
   <si>
     <t>error</t>
   </si>
   <si>
-    <t>Measured1</t>
+    <t>After Optimization
+Calculated</t>
   </si>
   <si>
     <t>Pose1_000</t>
@@ -63,6 +65,9 @@
   </si>
   <si>
     <t>Pose9_-9-90</t>
+  </si>
+  <si>
+    <t>Avg error</t>
   </si>
   <si>
     <t>a</t>
@@ -94,9 +99,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -109,7 +114,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,21 +158,77 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,91 +242,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,15 +250,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,7 +266,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,31 +326,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,91 +416,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,24 +440,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -430,24 +447,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,6 +591,30 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,54 +630,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,6 +660,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -701,10 +700,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -713,137 +712,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -853,14 +852,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -868,7 +873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
@@ -881,6 +886,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -942,6 +953,62 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="右箭头 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5048250" y="2174875"/>
+          <a:ext cx="869950" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1202,46 +1269,50 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="12.9090909090909" customWidth="1"/>
     <col min="5" max="5" width="10.6363636363636" customWidth="1"/>
-    <col min="6" max="6" width="11.8181818181818" customWidth="1"/>
-    <col min="8" max="8" width="10.6363636363636" customWidth="1"/>
+    <col min="6" max="6" width="13.3636363636364" customWidth="1"/>
+    <col min="8" max="8" width="13.2727272727273" customWidth="1"/>
+    <col min="9" max="9" width="10.6363636363636" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" ht="42" spans="1:9">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="6" t="s">
+      <c r="I1" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1">
@@ -1256,19 +1327,23 @@
       <c r="E2" s="2">
         <v>0.212</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="9">
         <v>0.2047</v>
       </c>
       <c r="G2">
         <f>ABS(E2-F2)</f>
         <v>0.0073</v>
       </c>
-      <c r="H2" s="8">
-        <v>0.198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
+      <c r="H2" s="10">
+        <v>0.212</v>
+      </c>
+      <c r="I2" s="16">
+        <f>ABS(E2-H2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1">
@@ -1283,19 +1358,23 @@
       <c r="E3" s="2">
         <v>0.115</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="9">
         <v>0.1095</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G10" si="0">ABS(E3-F3)</f>
         <v>0.0055</v>
       </c>
-      <c r="H3" s="8">
-        <v>0.107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
+      <c r="H3" s="10">
+        <v>0.115</v>
+      </c>
+      <c r="I3" s="16">
+        <f t="shared" ref="I3:I10" si="1">ABS(E3-H3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1">
@@ -1310,19 +1389,23 @@
       <c r="E4" s="2">
         <v>0.233</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="9">
         <v>0.2273</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
         <v>0.00570000000000001</v>
       </c>
-      <c r="H4" s="8">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="6" t="s">
+      <c r="H4" s="10">
+        <v>0.2326</v>
+      </c>
+      <c r="I4" s="16">
+        <f t="shared" si="1"/>
+        <v>0.000400000000000011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="1">
@@ -1337,19 +1420,23 @@
       <c r="E5" s="2">
         <v>0.118</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="9">
         <v>0.1119</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
         <v>0.00609999999999999</v>
       </c>
-      <c r="H5" s="8">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="6" t="s">
+      <c r="H5" s="10">
+        <v>0.118</v>
+      </c>
+      <c r="I5" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1">
@@ -1364,19 +1451,23 @@
       <c r="E6" s="2">
         <v>0.087</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="9">
         <v>0.07868</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
         <v>0.00831999999999999</v>
       </c>
-      <c r="H6" s="8">
-        <v>0.075</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
+      <c r="H6" s="10">
+        <v>0.087</v>
+      </c>
+      <c r="I6" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1">
@@ -1391,19 +1482,23 @@
       <c r="E7" s="2">
         <v>0.136</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="9">
         <v>0.1296</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
         <v>0.00640000000000002</v>
       </c>
-      <c r="H7" s="8">
-        <v>0.136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
+      <c r="H7" s="10">
+        <v>0.1362</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" si="1"/>
+        <v>0.000199999999999978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1">
@@ -1418,19 +1513,23 @@
       <c r="E8" s="2">
         <v>0.264</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="9">
         <v>0.2576</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
         <v>0.00640000000000002</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="10">
         <v>0.264</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
+      <c r="I8" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1">
@@ -1445,53 +1544,69 @@
       <c r="E9" s="2">
         <v>0.175</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="9">
         <v>0.1759</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
         <v>0.000900000000000012</v>
       </c>
-      <c r="H9" s="8">
-        <v>0.175</v>
-      </c>
-    </row>
-    <row r="10" ht="14.75" spans="1:8">
-      <c r="A10" s="9" t="s">
+      <c r="H9" s="10">
+        <v>0.1828</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="1"/>
+        <v>0.0078</v>
+      </c>
+    </row>
+    <row r="10" ht="14.75" spans="1:9">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="12">
         <v>-90</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="12">
         <v>-90</v>
       </c>
-      <c r="D10" s="10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="D10" s="12">
+        <v>0</v>
+      </c>
+      <c r="E10" s="13">
         <v>0.231</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="14">
         <v>0.2292</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
         <v>0.00180000000000002</v>
       </c>
-      <c r="H10" s="8">
-        <v>0.237</v>
-      </c>
-    </row>
-    <row r="11" spans="7:7">
+      <c r="H10" s="10">
+        <v>0.2313</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="1"/>
+        <v>0.000299999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="6:9">
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
       <c r="G11">
         <f>AVERAGE(G2:G10)</f>
         <v>0.00538000000000001</v>
       </c>
+      <c r="I11">
+        <f>AVERAGE(I2:I10)</f>
+        <v>0.000966666666666665</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1509,22 +1624,22 @@
     <row r="1" spans="1:7">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1598,7 +1713,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8">
         <f>C9/E9</f>
@@ -1632,7 +1747,7 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>2.2</v>

</xml_diff>

<commit_message>
fix some issues about update DH parameters added some callback functions
</commit_message>
<xml_diff>
--- a/Distance measurements.xlsx
+++ b/Distance measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7130"/>
+    <workbookView windowWidth="19200" windowHeight="7130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Distance Measurements" sheetId="1" r:id="rId1"/>
@@ -99,10 +99,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -114,9 +114,108 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -128,105 +227,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -251,7 +251,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,55 +266,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,31 +428,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,91 +446,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,30 +591,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,6 +637,30 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -700,10 +700,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -712,36 +712,36 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -751,98 +751,98 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -873,9 +873,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -886,12 +883,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1271,8 +1262,8 @@
   <sheetPr/>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -1307,7 +1298,7 @@
       <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1334,10 +1325,10 @@
         <f>ABS(E2-F2)</f>
         <v>0.0073</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="1">
         <v>0.212</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="2">
         <f>ABS(E2-H2)</f>
         <v>0</v>
       </c>
@@ -1365,10 +1356,10 @@
         <f t="shared" ref="G3:G10" si="0">ABS(E3-F3)</f>
         <v>0.0055</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="1">
         <v>0.115</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="2">
         <f t="shared" ref="I3:I10" si="1">ABS(E3-H3)</f>
         <v>0</v>
       </c>
@@ -1396,10 +1387,10 @@
         <f t="shared" si="0"/>
         <v>0.00570000000000001</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="1">
         <v>0.2326</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="2">
         <f t="shared" si="1"/>
         <v>0.000400000000000011</v>
       </c>
@@ -1427,10 +1418,10 @@
         <f t="shared" si="0"/>
         <v>0.00609999999999999</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="1">
         <v>0.118</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1458,10 +1449,10 @@
         <f t="shared" si="0"/>
         <v>0.00831999999999999</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="1">
         <v>0.087</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1489,10 +1480,10 @@
         <f t="shared" si="0"/>
         <v>0.00640000000000002</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="1">
         <v>0.1362</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="2">
         <f t="shared" si="1"/>
         <v>0.000199999999999978</v>
       </c>
@@ -1520,10 +1511,10 @@
         <f t="shared" si="0"/>
         <v>0.00640000000000002</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="1">
         <v>0.264</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1551,41 +1542,41 @@
         <f t="shared" si="0"/>
         <v>0.000900000000000012</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="1">
         <v>0.1828</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="2">
         <f t="shared" si="1"/>
         <v>0.0078</v>
       </c>
     </row>
     <row r="10" ht="14.75" spans="1:9">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>-90</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>-90</v>
       </c>
-      <c r="D10" s="12">
-        <v>0</v>
-      </c>
-      <c r="E10" s="13">
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12">
         <v>0.231</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>0.2292</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
         <v>0.00180000000000002</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="1">
         <v>0.2313</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="2">
         <f t="shared" si="1"/>
         <v>0.000299999999999995</v>
       </c>
@@ -1615,8 +1606,8 @@
   <sheetPr/>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -1653,16 +1644,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>0.047</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="F2" s="1">
-        <v>-120</v>
+        <v>-90</v>
       </c>
       <c r="G2" s="1">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1679,7 +1670,7 @@
         <v>0.02</v>
       </c>
       <c r="E3" s="1">
-        <v>16.8</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <v>-120</v>

</xml_diff>